<commit_message>
Updates to project outline and HCP ontology
</commit_message>
<xml_diff>
--- a/hcp_cognitive_ontology.xlsx
+++ b/hcp_cognitive_ontology.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t xml:space="preserve">Task/contrast description </t>
   </si>
@@ -94,13 +94,82 @@
   </si>
   <si>
     <t xml:space="preserve">Task </t>
+  </si>
+  <si>
+    <t>Recognition Memory</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Language Processing</t>
+  </si>
+  <si>
+    <t>Social Cognition</t>
+  </si>
+  <si>
+    <t>Relational Processing</t>
+  </si>
+  <si>
+    <t>Emotion Processing</t>
+  </si>
+  <si>
+    <t>Working Memory (O-Back)</t>
+  </si>
+  <si>
+    <t>Working Memory(2-Back)</t>
+  </si>
+  <si>
+    <t>Looking at images of bodies/faces/places/tools. Cued to look for image repeats with a different image in between.</t>
+  </si>
+  <si>
+    <t>Looking at images of bodies/faces/places/tools. Cued before task to look for a specific category. 2s pres / .5s ITI</t>
+  </si>
+  <si>
+    <t>0-back Con, 2-back Con, WM Con (2-back minus 0-back), Stim Grouop Cons, Targets, Non-Targets, Lures</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>not clear if pictures are at a location</t>
+  </si>
+  <si>
+    <t>not clear if pictures are at the same location</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Stimulus Modality</t>
+  </si>
+  <si>
+    <t>Explicit Stimulus</t>
+  </si>
+  <si>
+    <t>Stimulus Role</t>
+  </si>
+  <si>
+    <t>Response Modality</t>
+  </si>
+  <si>
+    <t>Overt Response</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>visual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -149,8 +218,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="URWPalladioL"/>
     </font>
@@ -163,7 +239,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -193,6 +269,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -215,7 +302,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -225,7 +312,11 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -577,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC27"/>
+  <dimension ref="A1:AN29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -588,28 +679,28 @@
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" customWidth="1"/>
+    <col min="16" max="16" width="14.5" customWidth="1"/>
     <col min="18" max="18" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.83203125" customWidth="1"/>
     <col min="20" max="20" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14" customWidth="1"/>
+    <col min="23" max="23" width="10.5" customWidth="1"/>
+    <col min="24" max="24" width="13.5" customWidth="1"/>
+    <col min="25" max="25" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="4" customFormat="1" ht="77" customHeight="1">
+    <row r="1" spans="1:40" s="4" customFormat="1" ht="77" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>24</v>
       </c>
@@ -619,247 +710,357 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" ht="90" customHeight="1">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:25" ht="60" customHeight="1">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:25" ht="75" customHeight="1">
+      <c r="Z1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
+      <c r="AK1" s="6"/>
+      <c r="AL1" s="6"/>
+      <c r="AM1" s="6"/>
+      <c r="AN1" s="6"/>
+    </row>
+    <row r="2" spans="1:40" ht="73" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" ht="73" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" ht="61" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:25" ht="60" customHeight="1">
-      <c r="A5" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" ht="122" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:25" ht="45" customHeight="1">
-      <c r="A6" s="1"/>
+    <row r="6" spans="1:40" ht="122" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:25" ht="60" customHeight="1">
-      <c r="A7" s="1"/>
+    <row r="7" spans="1:40" ht="122" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:25" ht="90" customHeight="1">
-      <c r="A8" s="1"/>
+    <row r="8" spans="1:40" ht="122" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:25" ht="75" customHeight="1">
-      <c r="A9" s="1"/>
+    <row r="9" spans="1:40" ht="122" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:25" ht="60" customHeight="1">
-      <c r="A10" s="1"/>
+    <row r="10" spans="1:40" ht="122" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-    </row>
-    <row r="11" spans="1:25" ht="75" customHeight="1">
+    </row>
+    <row r="11" spans="1:40" ht="75" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:25" ht="60" customHeight="1">
+    <row r="12" spans="1:40" ht="60" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:25" ht="75" customHeight="1">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+    </row>
+    <row r="13" spans="1:40" ht="75" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:25" ht="60" customHeight="1">
+    <row r="14" spans="1:40" ht="60" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:25" ht="75" customHeight="1">
+    <row r="15" spans="1:40" ht="75" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:25" ht="75" customHeight="1">
+    <row r="16" spans="1:40" ht="60" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:29" ht="60" customHeight="1">
+    <row r="17" spans="1:29" ht="75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:29" ht="60" customHeight="1">
+    <row r="18" spans="1:29" ht="75" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:29" ht="75" customHeight="1">
+    <row r="19" spans="1:29" ht="60" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:29" ht="90" customHeight="1">
+    <row r="20" spans="1:29" ht="60" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:29" ht="105" customHeight="1">
+    <row r="21" spans="1:29" ht="75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
-      <c r="X21" s="2"/>
-      <c r="Y21" s="2"/>
-      <c r="Z21" s="2"/>
-      <c r="AA21" s="2"/>
-      <c r="AB21" s="2"/>
-      <c r="AC21" s="2"/>
-    </row>
-    <row r="22" spans="1:29" ht="60" customHeight="1">
+    </row>
+    <row r="22" spans="1:29" ht="90" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:29" ht="60" customHeight="1">
+    <row r="23" spans="1:29" ht="105" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
     </row>
     <row r="24" spans="1:29" ht="60" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:29" ht="90" customHeight="1">
+    <row r="25" spans="1:29" ht="60" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:29" ht="90" customHeight="1">
+    <row r="26" spans="1:29" ht="60" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:29" ht="135" customHeight="1">
+    <row r="27" spans="1:29" ht="90" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:29" ht="90" customHeight="1">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:29" ht="135" customHeight="1">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Lots of updates to ontology
</commit_message>
<xml_diff>
--- a/hcp_cognitive_ontology.xlsx
+++ b/hcp_cognitive_ontology.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="38400" windowHeight="24000" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="38320" windowHeight="21840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
   <si>
     <t xml:space="preserve">Task/contrast description </t>
   </si>
@@ -163,13 +163,303 @@
   </si>
   <si>
     <t>visual</t>
+  </si>
+  <si>
+    <t>pictures</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>hand</t>
+  </si>
+  <si>
+    <t>button press</t>
+  </si>
+  <si>
+    <t>fixate, attend</t>
+  </si>
+  <si>
+    <t>fixate, attend, recall</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Localizer (Drobyshevsky </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">et al. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">2006); Reliable across subjects (Drobyshevsky </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">et al. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">2006) and time (Caceres </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">. 2009) </t>
+    </r>
+  </si>
+  <si>
+    <t>also, Faces, Places, Tools and Body Parts: Localizer (Downing et al. 2001; Peelen and Downing 2005; Taylor et al. 2007; Fox et al. 2009); Reliable across subjects (Downing et al. 2001; Fox et al. 2009) and time (Peelen and Downing 2005; Kung et al. 2007)</t>
+  </si>
+  <si>
+    <t>After working memory task, can be used to generate event-related contrasts for RECOGNIZED (remember or know) or NEW ITEM for items from the WM task.</t>
+  </si>
+  <si>
+    <t>Not sure how to deal with this task</t>
+  </si>
+  <si>
+    <t>Gambling</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Reliable across subjects and robust activation in fMRI (Delgado </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">. 2000; May </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">. 2004; Tricomi </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">. 2004; Forbes </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">. 2009) </t>
+    </r>
+  </si>
+  <si>
+    <t>Participants win lose money on gambling (+$1 or -$.5). Participants bet whether a card (value 1-&gt;9) is &gt;5 or &lt;5. Trials marked as reward/loss/neutral trials Event design, ? Instruction (1.5s) followed by feedback (1.0s), and ITI (1.0s). Always fixating. Blocked by # of reward/loss/neutral trials out of 8. (6/1/1, 6/0/2, 6/2/0 or (1/6/1, 0/6/2, 2/6/0). Each run has 2x mostly reward, 2x mostly loss interleaved with fixation.</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>symbols, digits</t>
+  </si>
+  <si>
+    <t>feedback</t>
+  </si>
+  <si>
+    <t>generate</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Fixation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Localizer (Morioka </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">. 1995; Bizzi </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">. 2008; Buckner </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">. 2011; Yeo </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">. 2011). </t>
+    </r>
+  </si>
+  <si>
+    <t>Movements blocked for 12s (10 moves) of left/right finger, toes, and tongue movements. Each pair of runs has 13 blocks (2 tongue, 2RH, 2LH, 2RF, 2LF) with 3 fixation blocks. Contrasts are movement - fixation.</t>
+  </si>
+  <si>
+    <t>shapes</t>
+  </si>
+  <si>
+    <t>hand/foot/mouth</t>
+  </si>
+  <si>
+    <t>flexion or extension</t>
+  </si>
+  <si>
+    <t>detect, move</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Reliable across subjects and robust activation (Binder </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">et al. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">2011). </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -229,6 +519,17 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="URWPalladioL"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ArialMT"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -302,7 +603,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -317,6 +618,19 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -668,39 +982,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN29"/>
+  <dimension ref="A1:AO30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" customWidth="1"/>
-    <col min="8" max="8" width="9.5" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" customWidth="1"/>
-    <col min="16" max="16" width="14.5" customWidth="1"/>
-    <col min="18" max="18" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.83203125" customWidth="1"/>
-    <col min="20" max="20" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14" customWidth="1"/>
-    <col min="23" max="23" width="10.5" customWidth="1"/>
-    <col min="24" max="24" width="13.5" customWidth="1"/>
-    <col min="25" max="25" width="11.1640625" customWidth="1"/>
+    <col min="3" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" customWidth="1"/>
+    <col min="9" max="9" width="9.5" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" customWidth="1"/>
+    <col min="17" max="17" width="14.5" customWidth="1"/>
+    <col min="19" max="19" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.83203125" customWidth="1"/>
+    <col min="21" max="21" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14" customWidth="1"/>
+    <col min="24" max="24" width="10.5" customWidth="1"/>
+    <col min="25" max="25" width="13.5" customWidth="1"/>
+    <col min="26" max="26" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="4" customFormat="1" ht="77" customHeight="1">
+    <row r="1" spans="1:41" s="4" customFormat="1" ht="77" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>24</v>
       </c>
@@ -710,91 +1024,93 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AF1" s="6"/>
       <c r="AG1" s="6"/>
       <c r="AH1" s="6"/>
       <c r="AI1" s="6"/>
@@ -803,37 +1119,56 @@
       <c r="AL1" s="6"/>
       <c r="AM1" s="6"/>
       <c r="AN1" s="6"/>
-    </row>
-    <row r="2" spans="1:40" ht="73" customHeight="1">
+      <c r="AO1" s="6"/>
+    </row>
+    <row r="2" spans="1:41" ht="73" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>40</v>
       </c>
-      <c r="M2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O2" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="N2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:40" ht="73" customHeight="1">
+      <c r="AB2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" ht="73" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -841,37 +1176,55 @@
         <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>40</v>
       </c>
-      <c r="M3" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S3" t="s">
-        <v>37</v>
-      </c>
-      <c r="V3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y3" t="s">
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W3" t="s">
         <v>37</v>
       </c>
       <c r="Z3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:40" ht="61" customHeight="1">
+      <c r="AB3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" ht="61" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>35</v>
@@ -879,188 +1232,321 @@
       <c r="C4" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:40" ht="122" customHeight="1">
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:41" ht="122" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:40" ht="122" customHeight="1">
+      <c r="B5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="Z5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" ht="122" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>65</v>
+      </c>
+      <c r="L6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" t="s">
+        <v>37</v>
+      </c>
+      <c r="P6" t="s">
+        <v>37</v>
+      </c>
+      <c r="R6" t="s">
+        <v>37</v>
+      </c>
+      <c r="S6" t="s">
+        <v>37</v>
+      </c>
+      <c r="T6" t="s">
+        <v>37</v>
+      </c>
+      <c r="U6" t="s">
+        <v>37</v>
+      </c>
+      <c r="V6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" ht="122" customHeight="1">
+      <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:40" ht="122" customHeight="1">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" ht="122" customHeight="1">
+      <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:40" ht="122" customHeight="1">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:41" ht="122" customHeight="1">
+      <c r="A9" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:40" ht="122" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:40" ht="122" customHeight="1">
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:41" ht="122" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:40" ht="75" customHeight="1">
-      <c r="A11" s="1"/>
+      <c r="D10" s="11"/>
+    </row>
+    <row r="11" spans="1:41" ht="122" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:40" ht="60" customHeight="1">
+      <c r="D11" s="11"/>
+    </row>
+    <row r="12" spans="1:41" ht="75" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-    </row>
-    <row r="13" spans="1:40" ht="75" customHeight="1">
+      <c r="D12" s="11"/>
+    </row>
+    <row r="13" spans="1:41" ht="60" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:40" ht="60" customHeight="1">
+      <c r="D13" s="11"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+    </row>
+    <row r="14" spans="1:41" ht="75" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:40" ht="75" customHeight="1">
+      <c r="D14" s="11"/>
+    </row>
+    <row r="15" spans="1:41" ht="60" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:40" ht="60" customHeight="1">
+      <c r="D15" s="11"/>
+    </row>
+    <row r="16" spans="1:41" ht="75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:29" ht="75" customHeight="1">
+      <c r="D16" s="11"/>
+    </row>
+    <row r="17" spans="1:30" ht="60" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:29" ht="75" customHeight="1">
+      <c r="D17" s="11"/>
+    </row>
+    <row r="18" spans="1:30" ht="75" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:29" ht="60" customHeight="1">
+      <c r="D18" s="11"/>
+    </row>
+    <row r="19" spans="1:30" ht="75" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:29" ht="60" customHeight="1">
+      <c r="D19" s="11"/>
+    </row>
+    <row r="20" spans="1:30" ht="60" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:29" ht="75" customHeight="1">
+      <c r="D20" s="11"/>
+    </row>
+    <row r="21" spans="1:30" ht="60" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:29" ht="90" customHeight="1">
+      <c r="D21" s="11"/>
+    </row>
+    <row r="22" spans="1:30" ht="75" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:29" ht="105" customHeight="1">
+      <c r="D22" s="11"/>
+    </row>
+    <row r="23" spans="1:30" ht="90" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
-      <c r="W23" s="2"/>
-      <c r="X23" s="2"/>
-      <c r="Y23" s="2"/>
-      <c r="Z23" s="2"/>
-      <c r="AA23" s="2"/>
-      <c r="AB23" s="2"/>
-      <c r="AC23" s="2"/>
-    </row>
-    <row r="24" spans="1:29" ht="60" customHeight="1">
+      <c r="D23" s="11"/>
+    </row>
+    <row r="24" spans="1:30" ht="105" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:29" ht="60" customHeight="1">
+      <c r="D24" s="11"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+    </row>
+    <row r="25" spans="1:30" ht="60" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:29" ht="60" customHeight="1">
+      <c r="D25" s="11"/>
+    </row>
+    <row r="26" spans="1:30" ht="60" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:29" ht="90" customHeight="1">
+      <c r="D26" s="11"/>
+    </row>
+    <row r="27" spans="1:30" ht="60" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:29" ht="90" customHeight="1">
+      <c r="D27" s="11"/>
+    </row>
+    <row r="28" spans="1:30" ht="90" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:29" ht="135" customHeight="1">
+      <c r="D28" s="11"/>
+    </row>
+    <row r="29" spans="1:30" ht="90" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
+      <c r="D29" s="11"/>
+    </row>
+    <row r="30" spans="1:30" ht="135" customHeight="1">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added missing openfmri tasks
</commit_message>
<xml_diff>
--- a/hcp_cognitive_ontology.xlsx
+++ b/hcp_cognitive_ontology.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="38320" windowHeight="21840" tabRatio="500"/>
+    <workbookView xWindow="40" yWindow="20" windowWidth="38320" windowHeight="21840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="148">
   <si>
     <t xml:space="preserve">Task/contrast description </t>
   </si>
@@ -630,6 +630,51 @@
   </si>
   <si>
     <t xml:space="preserve">Uncapher et al. (2011) </t>
+  </si>
+  <si>
+    <t>Task Num / Contrast Num</t>
+  </si>
+  <si>
+    <t>ds105</t>
+  </si>
+  <si>
+    <t>ds009</t>
+  </si>
+  <si>
+    <t>ds113</t>
+  </si>
+  <si>
+    <t>ds114</t>
+  </si>
+  <si>
+    <t>ds115</t>
+  </si>
+  <si>
+    <t>ds116</t>
+  </si>
+  <si>
+    <t>ds117</t>
+  </si>
+  <si>
+    <t>ds122</t>
+  </si>
+  <si>
+    <t>ds131</t>
+  </si>
+  <si>
+    <t>ds133</t>
+  </si>
+  <si>
+    <t>ds138</t>
+  </si>
+  <si>
+    <t>ds140</t>
+  </si>
+  <si>
+    <t>ds142</t>
+  </si>
+  <si>
+    <t>ds144</t>
   </si>
 </sst>
 </file>
@@ -759,8 +804,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -811,7 +866,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -821,6 +876,11 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -830,6 +890,11 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1159,136 +1224,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO37"/>
+  <dimension ref="A1:AP51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" customWidth="1"/>
-    <col min="9" max="9" width="9.5" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.6640625" customWidth="1"/>
-    <col min="17" max="17" width="14.5" customWidth="1"/>
-    <col min="19" max="19" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.83203125" customWidth="1"/>
-    <col min="21" max="21" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14" customWidth="1"/>
-    <col min="24" max="24" width="10.5" customWidth="1"/>
-    <col min="25" max="25" width="13.5" customWidth="1"/>
-    <col min="26" max="26" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="4" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" customWidth="1"/>
+    <col min="10" max="10" width="9.5" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" customWidth="1"/>
+    <col min="18" max="18" width="14.5" customWidth="1"/>
+    <col min="20" max="20" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.83203125" customWidth="1"/>
+    <col min="22" max="22" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14" customWidth="1"/>
+    <col min="25" max="25" width="10.5" customWidth="1"/>
+    <col min="26" max="26" width="13.5" customWidth="1"/>
+    <col min="27" max="27" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="4" customFormat="1" ht="77" customHeight="1">
+    <row r="1" spans="1:42" s="4" customFormat="1" ht="77" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AG1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AG1" s="6"/>
       <c r="AH1" s="6"/>
       <c r="AI1" s="6"/>
       <c r="AJ1" s="6"/>
@@ -1297,161 +1366,159 @@
       <c r="AM1" s="6"/>
       <c r="AN1" s="6"/>
       <c r="AO1" s="6"/>
-    </row>
-    <row r="2" spans="1:41" ht="73" customHeight="1">
+      <c r="AP1" s="6"/>
+    </row>
+    <row r="2" spans="1:42" ht="73" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>40</v>
       </c>
-      <c r="N2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P2" t="s">
-        <v>37</v>
-      </c>
-      <c r="T2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA2" t="s">
+      <c r="O2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB2" t="s">
         <v>47</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>48</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>49</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>50</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>51</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:41" ht="73" customHeight="1">
+    <row r="3" spans="1:42" ht="73" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>40</v>
       </c>
-      <c r="N3" t="s">
-        <v>37</v>
-      </c>
-      <c r="P3" t="s">
-        <v>37</v>
-      </c>
-      <c r="T3" t="s">
-        <v>37</v>
-      </c>
-      <c r="W3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z3" t="s">
+      <c r="O3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" t="s">
         <v>37</v>
       </c>
       <c r="AA3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB3" t="s">
         <v>47</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>48</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>49</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>50</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>51</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:41" ht="61" customHeight="1">
+    <row r="4" spans="1:42" ht="61" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="11"/>
-    </row>
-    <row r="5" spans="1:41" ht="122" customHeight="1">
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:42" ht="122" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="Z5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:41" ht="122" customHeight="1">
+      <c r="E5" s="11"/>
+      <c r="AA5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" ht="122" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="E6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
         <v>65</v>
       </c>
-      <c r="L6" t="s">
-        <v>37</v>
-      </c>
-      <c r="N6" t="s">
-        <v>37</v>
-      </c>
-      <c r="P6" t="s">
-        <v>37</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="M6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q6" t="s">
         <v>37</v>
       </c>
       <c r="S6" t="s">
@@ -1466,45 +1533,45 @@
       <c r="V6" t="s">
         <v>37</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="W6" t="s">
         <v>37</v>
       </c>
       <c r="AA6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB6" t="s">
         <v>61</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>62</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>63</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>50</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>51</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:41" ht="122" customHeight="1">
+    <row r="7" spans="1:42" ht="122" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="E7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>37</v>
       </c>
       <c r="O7" t="s">
@@ -1513,60 +1580,63 @@
       <c r="P7" t="s">
         <v>37</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="Q7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB7" t="s">
         <v>47</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>69</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>49</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>70</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>71</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AG7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:41" ht="122" customHeight="1">
+    <row r="8" spans="1:42" ht="122" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:41" ht="122" customHeight="1">
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:42" ht="122" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" spans="1:41" ht="122" customHeight="1">
+      <c r="D9" s="1"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:42" ht="122" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:41" ht="122" customHeight="1">
+      <c r="D10" s="1"/>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:42" ht="122" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="11"/>
-    </row>
-    <row r="12" spans="1:41" ht="75" customHeight="1">
+      <c r="D11" s="1"/>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:42" ht="75" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>74</v>
       </c>
@@ -1580,13 +1650,11 @@
         <v>76</v>
       </c>
       <c r="E12" s="11"/>
-      <c r="L12">
-        <v>1</v>
-      </c>
+      <c r="F12" s="11"/>
       <c r="M12">
         <v>1</v>
       </c>
-      <c r="S12">
+      <c r="N12">
         <v>1</v>
       </c>
       <c r="T12">
@@ -1595,11 +1663,14 @@
       <c r="U12">
         <v>1</v>
       </c>
-      <c r="X12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:41" ht="60" customHeight="1">
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" ht="60" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>77</v>
       </c>
@@ -1613,10 +1684,8 @@
         <v>79</v>
       </c>
       <c r="E13" s="11"/>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="O13">
+      <c r="F13" s="11"/>
+      <c r="N13">
         <v>1</v>
       </c>
       <c r="P13">
@@ -1625,11 +1694,14 @@
       <c r="Q13">
         <v>1</v>
       </c>
-      <c r="U13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:41" ht="75" customHeight="1">
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" ht="75" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>77</v>
       </c>
@@ -1643,20 +1715,21 @@
         <v>79</v>
       </c>
       <c r="E14" s="11"/>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="O14">
+      <c r="F14" s="11"/>
+      <c r="I14">
         <v>1</v>
       </c>
       <c r="P14">
         <v>1</v>
       </c>
-      <c r="V14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:41" ht="60" customHeight="1">
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" ht="60" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>77</v>
       </c>
@@ -1670,20 +1743,21 @@
         <v>79</v>
       </c>
       <c r="E15" s="11"/>
-      <c r="O15">
-        <v>1</v>
-      </c>
+      <c r="F15" s="11"/>
       <c r="P15">
         <v>1</v>
       </c>
       <c r="Q15">
         <v>1</v>
       </c>
-      <c r="U15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:41" ht="75" customHeight="1">
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" ht="75" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>82</v>
       </c>
@@ -1697,23 +1771,24 @@
         <v>84</v>
       </c>
       <c r="E16" s="11"/>
-      <c r="H16">
-        <v>1</v>
-      </c>
+      <c r="F16" s="11"/>
       <c r="I16">
         <v>1</v>
       </c>
-      <c r="O16">
-        <v>1</v>
-      </c>
-      <c r="Q16">
-        <v>1</v>
-      </c>
-      <c r="U16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" ht="60" customHeight="1">
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" ht="60" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>85</v>
       </c>
@@ -1727,11 +1802,12 @@
         <v>87</v>
       </c>
       <c r="E17" s="11"/>
-      <c r="S17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30" ht="75" customHeight="1">
+      <c r="F17" s="11"/>
+      <c r="T17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" ht="75" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>88</v>
       </c>
@@ -1745,17 +1821,18 @@
         <v>90</v>
       </c>
       <c r="E18" s="11"/>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30" ht="75" customHeight="1">
+      <c r="F18" s="11"/>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" ht="75" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>91</v>
       </c>
@@ -1769,20 +1846,21 @@
         <v>93</v>
       </c>
       <c r="E19" s="11"/>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="O19">
-        <v>1</v>
-      </c>
-      <c r="Q19">
-        <v>1</v>
-      </c>
-      <c r="U19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" ht="60" customHeight="1">
+      <c r="F19" s="11"/>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" ht="60" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>91</v>
       </c>
@@ -1796,37 +1874,38 @@
         <v>93</v>
       </c>
       <c r="E20" s="11"/>
-      <c r="F20" s="2"/>
+      <c r="F20" s="11"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="2">
-        <v>1</v>
-      </c>
-      <c r="I20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2">
+        <v>1</v>
+      </c>
       <c r="J20" s="2"/>
-      <c r="K20" s="2">
-        <v>1</v>
-      </c>
-      <c r="L20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2">
+        <v>1</v>
+      </c>
       <c r="M20" s="2"/>
-      <c r="N20" s="2">
-        <v>1</v>
-      </c>
+      <c r="N20" s="2"/>
       <c r="O20" s="2">
         <v>1</v>
       </c>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2">
-        <v>1</v>
-      </c>
-      <c r="R20" s="2"/>
+      <c r="P20" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2">
+        <v>1</v>
+      </c>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
-    </row>
-    <row r="21" spans="1:30" ht="60" customHeight="1">
+      <c r="Y20" s="2"/>
+    </row>
+    <row r="21" spans="1:31" ht="60" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>91</v>
       </c>
@@ -1840,26 +1919,27 @@
         <v>93</v>
       </c>
       <c r="E21" s="11"/>
-      <c r="H21">
-        <v>1</v>
-      </c>
+      <c r="F21" s="11"/>
       <c r="I21">
         <v>1</v>
       </c>
-      <c r="K21">
-        <v>1</v>
-      </c>
-      <c r="N21">
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="L21">
         <v>1</v>
       </c>
       <c r="O21">
         <v>1</v>
       </c>
-      <c r="Q21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30" ht="75" customHeight="1">
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" ht="75" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>96</v>
       </c>
@@ -1873,20 +1953,21 @@
         <v>98</v>
       </c>
       <c r="E22" s="11"/>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="N22">
-        <v>1</v>
-      </c>
-      <c r="R22">
-        <v>1</v>
-      </c>
-      <c r="X22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30" ht="90" customHeight="1">
+      <c r="F22" s="11"/>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="Y22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" ht="90" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>96</v>
       </c>
@@ -1900,23 +1981,24 @@
         <v>98</v>
       </c>
       <c r="E23" s="11"/>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="R23">
-        <v>1</v>
-      </c>
-      <c r="U23">
-        <v>1</v>
-      </c>
-      <c r="X23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30" ht="105" customHeight="1">
+      <c r="F23" s="11"/>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="Y23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" ht="105" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>100</v>
       </c>
@@ -1930,17 +2012,18 @@
         <v>102</v>
       </c>
       <c r="E24" s="11"/>
-      <c r="L24">
-        <v>1</v>
-      </c>
-      <c r="N24">
-        <v>1</v>
-      </c>
-      <c r="AB24" s="2"/>
+      <c r="F24" s="11"/>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
       <c r="AC24" s="2"/>
       <c r="AD24" s="2"/>
-    </row>
-    <row r="25" spans="1:30" ht="60" customHeight="1">
+      <c r="AE24" s="2"/>
+    </row>
+    <row r="25" spans="1:31" ht="60" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>100</v>
       </c>
@@ -1954,10 +2037,8 @@
         <v>102</v>
       </c>
       <c r="E25" s="11"/>
-      <c r="M25">
-        <v>1</v>
-      </c>
-      <c r="O25">
+      <c r="F25" s="11"/>
+      <c r="N25">
         <v>1</v>
       </c>
       <c r="P25">
@@ -1966,11 +2047,14 @@
       <c r="Q25">
         <v>1</v>
       </c>
-      <c r="U25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:30" ht="60" customHeight="1">
+      <c r="R25">
+        <v>1</v>
+      </c>
+      <c r="V25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" ht="60" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>100</v>
       </c>
@@ -1984,10 +2068,8 @@
         <v>102</v>
       </c>
       <c r="E26" s="11"/>
-      <c r="G26">
-        <v>1</v>
-      </c>
-      <c r="L26">
+      <c r="F26" s="11"/>
+      <c r="H26">
         <v>1</v>
       </c>
       <c r="M26">
@@ -2005,14 +2087,17 @@
       <c r="Q26">
         <v>1</v>
       </c>
-      <c r="U26">
+      <c r="R26">
         <v>1</v>
       </c>
       <c r="V26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:30" ht="60" customHeight="1">
+      <c r="W26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" ht="60" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>100</v>
       </c>
@@ -2026,20 +2111,21 @@
         <v>102</v>
       </c>
       <c r="E27" s="11"/>
-      <c r="O27">
-        <v>1</v>
-      </c>
+      <c r="F27" s="11"/>
       <c r="P27">
         <v>1</v>
       </c>
       <c r="Q27">
         <v>1</v>
       </c>
-      <c r="U27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:30" ht="90" customHeight="1">
+      <c r="R27">
+        <v>1</v>
+      </c>
+      <c r="V27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" ht="90" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>105</v>
       </c>
@@ -2053,23 +2139,24 @@
         <v>107</v>
       </c>
       <c r="E28" s="11"/>
-      <c r="O28">
-        <v>1</v>
-      </c>
+      <c r="F28" s="11"/>
       <c r="P28">
         <v>1</v>
       </c>
       <c r="Q28">
         <v>1</v>
       </c>
-      <c r="U28">
-        <v>1</v>
-      </c>
-      <c r="X28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30" ht="90" customHeight="1">
+      <c r="R28">
+        <v>1</v>
+      </c>
+      <c r="V28">
+        <v>1</v>
+      </c>
+      <c r="Y28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" ht="90" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>108</v>
       </c>
@@ -2083,17 +2170,18 @@
         <v>110</v>
       </c>
       <c r="E29" s="11"/>
-      <c r="H29">
-        <v>1</v>
-      </c>
+      <c r="F29" s="11"/>
       <c r="I29">
         <v>1</v>
       </c>
       <c r="J29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:30" ht="135" customHeight="1">
+      <c r="K29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" ht="135" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>111</v>
       </c>
@@ -2107,23 +2195,24 @@
         <v>113</v>
       </c>
       <c r="E30" s="11"/>
-      <c r="H30">
-        <v>1</v>
-      </c>
-      <c r="O30">
+      <c r="F30" s="11"/>
+      <c r="I30">
         <v>1</v>
       </c>
       <c r="P30">
         <v>1</v>
       </c>
-      <c r="S30">
-        <v>1</v>
-      </c>
-      <c r="V30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:30" ht="75">
+      <c r="Q30">
+        <v>1</v>
+      </c>
+      <c r="T30">
+        <v>1</v>
+      </c>
+      <c r="W30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" ht="30">
       <c r="A31" s="1" t="s">
         <v>111</v>
       </c>
@@ -2137,40 +2226,41 @@
         <v>113</v>
       </c>
       <c r="E31" s="11"/>
-      <c r="F31" s="2"/>
+      <c r="F31" s="11"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="2">
-        <v>1</v>
-      </c>
-      <c r="I31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2">
+        <v>1</v>
+      </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
-      <c r="O31" s="2">
-        <v>1</v>
-      </c>
+      <c r="O31" s="2"/>
       <c r="P31" s="2">
         <v>1</v>
       </c>
-      <c r="Q31" s="2"/>
+      <c r="Q31" s="2">
+        <v>1</v>
+      </c>
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
-      <c r="T31" s="2">
-        <v>1</v>
-      </c>
-      <c r="U31" s="2"/>
-      <c r="V31" s="2">
-        <v>1</v>
-      </c>
-      <c r="W31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2">
+        <v>1</v>
+      </c>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2">
+        <v>1</v>
+      </c>
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
       <c r="AA31" s="2"/>
-    </row>
-    <row r="32" spans="1:30" ht="45">
+      <c r="AB31" s="2"/>
+    </row>
+    <row r="32" spans="1:31" ht="30">
       <c r="A32" s="1" t="s">
         <v>115</v>
       </c>
@@ -2184,11 +2274,12 @@
         <v>117</v>
       </c>
       <c r="E32" s="11"/>
-      <c r="W32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:27" ht="45">
+      <c r="F32" s="11"/>
+      <c r="X32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28">
       <c r="A33" s="1" t="s">
         <v>118</v>
       </c>
@@ -2202,14 +2293,15 @@
         <v>120</v>
       </c>
       <c r="E33" s="11"/>
-      <c r="R33">
-        <v>1</v>
-      </c>
-      <c r="X33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:27" ht="45">
+      <c r="F33" s="11"/>
+      <c r="S33">
+        <v>1</v>
+      </c>
+      <c r="Y33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" ht="30">
       <c r="A34" s="1" t="s">
         <v>121</v>
       </c>
@@ -2223,14 +2315,15 @@
         <v>123</v>
       </c>
       <c r="E34" s="11"/>
-      <c r="I34">
-        <v>1</v>
-      </c>
+      <c r="F34" s="11"/>
       <c r="J34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:27" ht="60">
+      <c r="K34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" ht="30">
       <c r="A35" s="1" t="s">
         <v>124</v>
       </c>
@@ -2244,11 +2337,12 @@
         <v>126</v>
       </c>
       <c r="E35" s="11"/>
-      <c r="Y35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:27" ht="60">
+      <c r="F35" s="11"/>
+      <c r="Z35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" ht="30">
       <c r="A36" s="1" t="s">
         <v>127</v>
       </c>
@@ -2262,11 +2356,12 @@
         <v>129</v>
       </c>
       <c r="E36" s="11"/>
-      <c r="Z36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27" ht="75">
+      <c r="F36" s="11"/>
+      <c r="AA36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" ht="30">
       <c r="A37" s="1" t="s">
         <v>130</v>
       </c>
@@ -2280,8 +2375,79 @@
         <v>132</v>
       </c>
       <c r="E37" s="11"/>
-      <c r="AA37">
-        <v>1</v>
+      <c r="F37" s="11"/>
+      <c r="AB37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28">
+      <c r="A38" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28">
+      <c r="A39" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28">
+      <c r="A40" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28">
+      <c r="A41" s="12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28">
+      <c r="A42" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28">
+      <c r="A43" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28">
+      <c r="A44" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28">
+      <c r="A45" s="12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28">
+      <c r="A46" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28">
+      <c r="A47" s="12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28">
+      <c r="A48" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="12" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New updates to hop ontology
</commit_message>
<xml_diff>
--- a/hcp_cognitive_ontology.xlsx
+++ b/hcp_cognitive_ontology.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="149">
   <si>
     <t xml:space="preserve">Task/contrast description </t>
   </si>
@@ -675,6 +675,9 @@
   </si>
   <si>
     <t>ds144</t>
+  </si>
+  <si>
+    <t>30 sec blocks in which participants listen to a brief story (5-9 sentences) from Aesop's, followed by a question about the topic. Math task presents oral trials asking participants to solve a math problem (e.g. "fourteen plus twelve", followed by two choices "twenty-nine or twenty-six")</t>
   </si>
 </sst>
 </file>
@@ -1227,7 +1230,7 @@
   <dimension ref="A1:AP51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1607,6 +1610,9 @@
         <v>27</v>
       </c>
       <c r="B8" s="1"/>
+      <c r="C8" s="5" t="s">
+        <v>148</v>
+      </c>
       <c r="D8" s="8" t="s">
         <v>73</v>
       </c>

</xml_diff>